<commit_message>
added testcase reading logic from excel
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataSheet1.xlsx
+++ b/src/test/java/dataEngine/DataSheet1.xlsx
@@ -7,23 +7,24 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
-    <sheet name="Test Steps" sheetId="1" r:id="rId2"/>
-    <sheet name="Test Data" sheetId="3" r:id="rId3"/>
-    <sheet name="Settings" sheetId="4" r:id="rId4"/>
+    <sheet name="FunctionalSuite" sheetId="2" r:id="rId1"/>
+    <sheet name="SmokeSuite" sheetId="5" r:id="rId2"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId3"/>
+    <sheet name="Test Data" sheetId="3" r:id="rId4"/>
+    <sheet name="ObjectRepo" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Action_Keywords">Settings!$D$2:$D$8</definedName>
-    <definedName name="Home_Page">Settings!$B$2:$B$8</definedName>
-    <definedName name="Login_Page">Settings!$C$2:$C$8</definedName>
-    <definedName name="Page_Name">Settings!$A$2:$A$8</definedName>
+    <definedName name="Action_Keywords">ObjectRepo!$D$2:$D$8</definedName>
+    <definedName name="Home_Page">ObjectRepo!$B$2:$B$8</definedName>
+    <definedName name="Login_Page">ObjectRepo!$C$2:$C$8</definedName>
+    <definedName name="Page_Name">ObjectRepo!$A$2:$A$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
@@ -61,15 +62,6 @@
     <t>TS_002</t>
   </si>
   <si>
-    <t>TS_004</t>
-  </si>
-  <si>
-    <t>TS_005</t>
-  </si>
-  <si>
-    <t>TS_006</t>
-  </si>
-  <si>
     <t>testuser_1</t>
   </si>
   <si>
@@ -97,15 +89,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Page Name</t>
   </si>
   <si>
-    <t>LogIn_Page Objects</t>
-  </si>
-  <si>
     <t>btn_MyAccount</t>
   </si>
   <si>
@@ -124,9 +110,6 @@
     <t>Action Keywords</t>
   </si>
   <si>
-    <t>input</t>
-  </si>
-  <si>
     <t>Home_Page</t>
   </si>
   <si>
@@ -139,15 +122,9 @@
     <t>Action Keyword</t>
   </si>
   <si>
-    <t>Data Set</t>
-  </si>
-  <si>
     <t>waitFor</t>
   </si>
   <si>
-    <t>testuser_3</t>
-  </si>
-  <si>
     <t>LogIn_02</t>
   </si>
   <si>
@@ -157,28 +134,79 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>INPUT textbox</t>
-  </si>
-  <si>
-    <t>click google search</t>
-  </si>
-  <si>
     <t>TS_003</t>
   </si>
   <si>
-    <t xml:space="preserve">WAIT </t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
     <t>press_enter</t>
   </si>
   <si>
-    <t>Google_Page Objects</t>
-  </si>
-  <si>
     <t>googleSearchBox</t>
+  </si>
+  <si>
+    <t>TS_001</t>
+  </si>
+  <si>
+    <t>debapriyo.halder@imerit.net</t>
+  </si>
+  <si>
+    <t>Page Objects</t>
+  </si>
+  <si>
+    <t>Page_Objects_Description</t>
+  </si>
+  <si>
+    <t>input_text</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Navigate to itest</t>
+  </si>
+  <si>
+    <t>Login to google account</t>
+  </si>
+  <si>
+    <t>googleLogin</t>
+  </si>
+  <si>
+    <t>click on Login to impp button</t>
+  </si>
+  <si>
+    <t>TestClass</t>
+  </si>
+  <si>
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>LogIn_03</t>
+  </si>
+  <si>
+    <t>LogIn_04</t>
+  </si>
+  <si>
+    <t>LogIn_05</t>
+  </si>
+  <si>
+    <t>LogIn_06</t>
   </si>
 </sst>
 </file>
@@ -210,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,8 +257,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -253,12 +299,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -270,6 +327,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -575,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +657,7 @@
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -599,34 +668,101 @@
         <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -636,10 +772,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +856,7 @@
     <col min="4" max="4" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="38.140625" customWidth="1" collapsed="1"/>
   </cols>
@@ -660,157 +866,181 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>38</v>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="G3" s="2" t="str">
         <f>'Test Data'!B2</f>
-        <v>testuser_3</v>
+        <v>debapriyo.halder@imerit.net</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="G4" s="2" t="str">
         <f>'Test Data'!C2</f>
         <v>Test@123</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2" t="str">
         <f>'Test Data'!C3</f>
         <v>Test@123</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7">
       <formula1>Page_Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7">
       <formula1>Action_Keywords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -819,17 +1049,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -843,35 +1075,35 @@
         <v>10</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,17 +1146,18 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,27 +1167,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -962,13 +1195,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -978,7 +1211,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
@@ -989,7 +1222,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,14 +1238,16 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added base 64 encryption
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataSheet1.xlsx
+++ b/src/test/java/dataEngine/DataSheet1.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FunctionalSuite" sheetId="2" r:id="rId1"/>
     <sheet name="SmokeSuite" sheetId="5" r:id="rId2"/>
-    <sheet name="Test Steps" sheetId="1" r:id="rId3"/>
+    <sheet name="Test Steps" sheetId="1" state="hidden" r:id="rId3"/>
     <sheet name="Test Data" sheetId="3" r:id="rId4"/>
-    <sheet name="ObjectRepo" sheetId="4" r:id="rId5"/>
+    <sheet name="ObjectRepo" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Action_Keywords">ObjectRepo!$D$2:$D$8</definedName>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>Description</t>
   </si>
@@ -65,9 +65,6 @@
     <t>testuser_1</t>
   </si>
   <si>
-    <t>Test@123</t>
-  </si>
-  <si>
     <t>Close the Browser</t>
   </si>
   <si>
@@ -207,13 +204,37 @@
   </si>
   <si>
     <t>LogIn_06</t>
+  </si>
+  <si>
+    <t>smk_01</t>
+  </si>
+  <si>
+    <t>smk_02</t>
+  </si>
+  <si>
+    <t>job_code</t>
+  </si>
+  <si>
+    <t>engagement_code</t>
+  </si>
+  <si>
+    <t>Test@123456</t>
+  </si>
+  <si>
+    <t>VGVzdEAxMjM=</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>asdsd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +254,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -315,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -339,6 +367,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -647,7 +678,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,100 +699,100 @@
         <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -774,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,42 +828,42 @@
         <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -866,59 +897,59 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
@@ -929,48 +960,48 @@
         <v>debapriyo.halder@imerit.net</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="2" t="str">
         <f>'Test Data'!C2</f>
-        <v>Test@123</v>
+        <v>VGVzdEAxMjM=</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
@@ -978,58 +1009,58 @@
       </c>
       <c r="G5" s="2" t="str">
         <f>'Test Data'!C3</f>
-        <v>Test@123</v>
+        <v>Test@123456</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1051,20 +1082,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -1075,80 +1108,93 @@
         <v>10</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
+      <c r="C3" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" display="Test@123"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1157,7 +1203,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,27 +1213,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -1195,13 +1241,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -1211,7 +1257,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
@@ -1222,7 +1268,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,7 +1284,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1246,7 +1292,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added dashboard tc and corrected keyword functions
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataSheet1.xlsx
+++ b/src/test/java/dataEngine/DataSheet1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="6885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FunctionalSuite" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>Description</t>
   </si>
@@ -176,9 +176,6 @@
     <t>TestClass</t>
   </si>
   <si>
-    <t>TC_001</t>
-  </si>
-  <si>
     <t>TC_002</t>
   </si>
   <si>
@@ -194,18 +191,6 @@
     <t>TC_006</t>
   </si>
   <si>
-    <t>LogIn_03</t>
-  </si>
-  <si>
-    <t>LogIn_04</t>
-  </si>
-  <si>
-    <t>LogIn_05</t>
-  </si>
-  <si>
-    <t>LogIn_06</t>
-  </si>
-  <si>
     <t>smk_01</t>
   </si>
   <si>
@@ -228,6 +213,36 @@
   </si>
   <si>
     <t>asdsd</t>
+  </si>
+  <si>
+    <t>chromes</t>
+  </si>
+  <si>
+    <t>Verification of dashboard</t>
+  </si>
+  <si>
+    <t>func_01</t>
+  </si>
+  <si>
+    <t>func_02</t>
+  </si>
+  <si>
+    <t>func_03</t>
+  </si>
+  <si>
+    <t>func_04</t>
+  </si>
+  <si>
+    <t>func_05</t>
+  </si>
+  <si>
+    <t>func_06</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>JC-ry2VIGx07</t>
   </si>
 </sst>
 </file>
@@ -678,7 +693,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,6 +701,7 @@
     <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="55.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -707,22 +723,22 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -732,12 +748,12 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -747,12 +763,12 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -762,12 +778,12 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -777,12 +793,12 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -792,7 +808,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +822,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +852,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -844,16 +860,14 @@
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -863,7 +877,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1099,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,6 +1108,7 @@
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.5703125" style="13" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1111,16 +1126,16 @@
         <v>18</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1131,10 +1146,13 @@
         <v>40</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1145,7 +1163,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>36</v>

</xml_diff>